<commit_message>
Updated notebooks to include Shap analysis of models.
</commit_message>
<xml_diff>
--- a/comparison.xlsx
+++ b/comparison.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Petter/Projects/TIP160/Facies-prediction-TIP160/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207DF493-995F-1C4B-9FE7-3809DCBBE7BA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D68CABF9-7CE6-1047-ADF4-4A82ED759413}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="16000" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="26" uniqueCount="18">
   <si>
     <t>Improvement in %</t>
   </si>
@@ -51,12 +51,48 @@
   </si>
   <si>
     <t>Løsning 3 vs. LA team</t>
+  </si>
+  <si>
+    <t>Løsning 1</t>
+  </si>
+  <si>
+    <t>Løsning 2</t>
+  </si>
+  <si>
+    <t>Løsning 3</t>
+  </si>
+  <si>
+    <t>F1-score</t>
+  </si>
+  <si>
+    <t>Avstand fra beste F1-score</t>
+  </si>
+  <si>
+    <t>Forbedring mot LA Team</t>
+  </si>
+  <si>
+    <t>-</t>
+  </si>
+  <si>
+    <t>Kompetansebehov</t>
+  </si>
+  <si>
+    <t>Høyt</t>
+  </si>
+  <si>
+    <t>Middels</t>
+  </si>
+  <si>
+    <t>Lavt</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="166" formatCode="0.000%"/>
+  </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -92,7 +128,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="12">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -135,8 +171,32 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFDC0"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -159,28 +219,102 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="17">
+  <cellXfs count="29">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" indent="1"/>
     </xf>
@@ -206,6 +340,51 @@
       <alignment horizontal="left" vertical="center" indent="3"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="11" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="10" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="11" borderId="2" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="8" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="9" borderId="6" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="7" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="6" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="9" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="8" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="166" fontId="0" fillId="11" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -215,6 +394,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFFFFDC0"/>
+      <color rgb="FFFFF9A8"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -511,225 +696,348 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:J21"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="111" workbookViewId="0">
-      <selection activeCell="B7" sqref="B7"/>
+    <sheetView tabSelected="1" topLeftCell="D1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="27.1640625" defaultRowHeight="20" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="23" customWidth="1"/>
     <col min="3" max="3" width="14.1640625" customWidth="1"/>
+    <col min="4" max="4" width="35.1640625" customWidth="1"/>
+    <col min="5" max="5" width="15.6640625" customWidth="1"/>
+    <col min="9" max="9" width="24.33203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:10" ht="28" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="1"/>
       <c r="D1" s="1"/>
-    </row>
-    <row r="2" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
+      <c r="H1" s="1"/>
+      <c r="I1" s="1"/>
+      <c r="J1" s="1"/>
+    </row>
+    <row r="2" spans="1:10" ht="21" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="16" t="s">
+      <c r="B2" s="13" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="16"/>
-      <c r="D2" s="6"/>
-      <c r="E2" s="7"/>
-      <c r="F2" s="7"/>
-    </row>
-    <row r="3" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="C2" s="13"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="16" t="s">
+        <v>10</v>
+      </c>
+      <c r="G2" s="16" t="s">
+        <v>12</v>
+      </c>
+      <c r="H2" s="16" t="s">
+        <v>11</v>
+      </c>
+      <c r="I2" s="17" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" s="1"/>
+    </row>
+    <row r="3" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="1"/>
-      <c r="B3" s="8" t="s">
+      <c r="B3" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C3" s="13">
+      <c r="C3" s="10">
         <v>0.68418072289156628</v>
       </c>
       <c r="D3" s="3"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-    </row>
-    <row r="4" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E3" s="18" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="14">
+        <v>0.68418072289156628</v>
+      </c>
+      <c r="G3" s="26">
+        <v>6.7364622295735102E-2</v>
+      </c>
+      <c r="H3" s="24">
+        <f>-(F4/F3-1)</f>
+        <v>-4.2704034374064337E-2</v>
+      </c>
+      <c r="I3" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="J3" s="1"/>
+    </row>
+    <row r="4" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="1"/>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C4" s="14">
+      <c r="C4" s="11">
         <v>0.64100000000000001</v>
       </c>
       <c r="D4" s="2"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E4" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="F4" s="14">
+        <v>0.71339799999999998</v>
+      </c>
+      <c r="G4" s="27">
+        <f>C9/C10-1</f>
+        <v>0.11294539781591251</v>
+      </c>
+      <c r="H4" s="25">
+        <f>-(F5/F4-1)</f>
+        <v>-1.330753137107199E-2</v>
+      </c>
+      <c r="I4" s="22" t="s">
+        <v>16</v>
+      </c>
+      <c r="J4" s="1"/>
+    </row>
+    <row r="5" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="1"/>
-      <c r="B5" s="9" t="s">
+      <c r="B5" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C5" s="11">
+      <c r="C5" s="8">
         <v>6.7364622295735102E-2</v>
       </c>
       <c r="D5" s="2"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E5" s="19" t="s">
+        <v>9</v>
+      </c>
+      <c r="F5" s="20">
+        <v>0.72289156626506001</v>
+      </c>
+      <c r="G5" s="28">
+        <f>C15/C16-1</f>
+        <v>0.12775595361163816</v>
+      </c>
+      <c r="H5" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="I5" s="23" t="s">
+        <v>17</v>
+      </c>
+      <c r="J5" s="1"/>
+    </row>
+    <row r="6" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1"/>
-      <c r="B6" s="10" t="s">
+      <c r="B6" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C6" s="15">
+      <c r="C6" s="12">
         <v>0.93455421686746998</v>
       </c>
       <c r="D6" s="2"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E6" s="3"/>
+      <c r="F6" s="2"/>
+      <c r="G6" s="2"/>
+      <c r="H6" s="2"/>
+      <c r="I6" s="2"/>
+      <c r="J6" s="1"/>
+    </row>
+    <row r="7" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1"/>
       <c r="B7" s="2"/>
       <c r="C7" s="2"/>
       <c r="D7" s="2"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E7" s="3"/>
+      <c r="F7" s="2"/>
+      <c r="G7" s="2"/>
+      <c r="H7" s="2"/>
+      <c r="I7" s="2"/>
+    </row>
+    <row r="8" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1"/>
-      <c r="B8" s="16" t="s">
+      <c r="B8" s="13" t="s">
         <v>5</v>
       </c>
-      <c r="C8" s="16"/>
+      <c r="C8" s="13"/>
       <c r="D8" s="2"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
-    </row>
-    <row r="9" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E8" s="3"/>
+      <c r="F8" s="2"/>
+      <c r="G8" s="2"/>
+      <c r="H8" s="2"/>
+      <c r="I8" s="2"/>
+    </row>
+    <row r="9" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1"/>
-      <c r="B9" s="8" t="s">
+      <c r="B9" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C9" s="13">
+      <c r="C9" s="10">
         <v>0.71339799999999998</v>
       </c>
       <c r="D9" s="2"/>
-      <c r="E9" s="5"/>
-      <c r="F9" s="5"/>
-    </row>
-    <row r="10" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E9" s="3"/>
+      <c r="F9" s="2"/>
+      <c r="G9" s="2"/>
+      <c r="H9" s="2"/>
+      <c r="I9" s="2"/>
+    </row>
+    <row r="10" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1"/>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C10" s="14">
+      <c r="C10" s="11">
         <v>0.64100000000000001</v>
       </c>
       <c r="D10" s="2"/>
-      <c r="E10" s="5"/>
-      <c r="F10" s="5"/>
-    </row>
-    <row r="11" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E10" s="3"/>
+      <c r="F10" s="2"/>
+      <c r="G10" s="2"/>
+      <c r="H10" s="2"/>
+      <c r="I10" s="2"/>
+    </row>
+    <row r="11" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="1"/>
-      <c r="B11" s="9" t="s">
+      <c r="B11" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C11" s="11">
+      <c r="C11" s="8">
         <f>C9/C10-1</f>
         <v>0.11294539781591251</v>
       </c>
       <c r="D11" s="2"/>
-      <c r="E11" s="5"/>
-      <c r="F11" s="5"/>
-    </row>
-    <row r="12" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E11" s="3"/>
+      <c r="F11" s="2"/>
+      <c r="G11" s="2"/>
+      <c r="H11" s="2"/>
+      <c r="I11" s="2"/>
+    </row>
+    <row r="12" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="1"/>
-      <c r="B12" s="10" t="s">
+      <c r="B12" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="15">
+      <c r="C12" s="12">
         <v>0.93015662650602404</v>
       </c>
       <c r="D12" s="2"/>
-      <c r="E12" s="5"/>
-      <c r="F12" s="5"/>
-    </row>
-    <row r="13" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E12" s="3"/>
+      <c r="F12" s="2"/>
+      <c r="G12" s="2"/>
+      <c r="H12" s="2"/>
+      <c r="I12" s="2"/>
+    </row>
+    <row r="13" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="1"/>
       <c r="B13" s="2"/>
       <c r="C13" s="2"/>
       <c r="D13" s="2"/>
-      <c r="E13" s="5"/>
-      <c r="F13" s="5"/>
-    </row>
-    <row r="14" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E13" s="3"/>
+      <c r="F13" s="2"/>
+      <c r="G13" s="2"/>
+      <c r="H13" s="2"/>
+      <c r="I13" s="2"/>
+    </row>
+    <row r="14" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="1"/>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="13" t="s">
         <v>6</v>
       </c>
-      <c r="C14" s="16"/>
+      <c r="C14" s="13"/>
       <c r="D14" s="2"/>
-      <c r="E14" s="5"/>
-      <c r="F14" s="5"/>
-    </row>
-    <row r="15" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E14" s="3"/>
+      <c r="F14" s="2"/>
+      <c r="G14" s="2"/>
+      <c r="H14" s="2"/>
+      <c r="I14" s="2"/>
+    </row>
+    <row r="15" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="1"/>
-      <c r="B15" s="8" t="s">
+      <c r="B15" s="5" t="s">
         <v>3</v>
       </c>
-      <c r="C15" s="13">
+      <c r="C15" s="10">
         <v>0.72289156626506001</v>
       </c>
       <c r="D15" s="2"/>
-    </row>
-    <row r="16" spans="1:6" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E15" s="3"/>
+      <c r="F15" s="2"/>
+      <c r="G15" s="2"/>
+      <c r="H15" s="2"/>
+      <c r="I15" s="2"/>
+    </row>
+    <row r="16" spans="1:10" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="1"/>
-      <c r="B16" s="12" t="s">
+      <c r="B16" s="9" t="s">
         <v>4</v>
       </c>
-      <c r="C16" s="14">
+      <c r="C16" s="11">
         <v>0.64100000000000001</v>
       </c>
       <c r="D16" s="2"/>
-    </row>
-    <row r="17" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E16" s="3"/>
+      <c r="F16" s="2"/>
+      <c r="G16" s="2"/>
+      <c r="H16" s="2"/>
+      <c r="I16" s="2"/>
+    </row>
+    <row r="17" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="1"/>
-      <c r="B17" s="9" t="s">
+      <c r="B17" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="11">
+      <c r="C17" s="8">
         <f>C15/C16-1</f>
         <v>0.12775595361163816</v>
       </c>
       <c r="D17" s="2"/>
-    </row>
-    <row r="18" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E17" s="2"/>
+      <c r="F17" s="2"/>
+      <c r="G17" s="2"/>
+      <c r="H17" s="2"/>
+    </row>
+    <row r="18" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="1"/>
-      <c r="B18" s="10" t="s">
+      <c r="B18" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="C18" s="15">
+      <c r="C18" s="12">
         <v>0.91325301204819198</v>
       </c>
       <c r="D18" s="2"/>
-    </row>
-    <row r="19" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E18" s="2"/>
+      <c r="F18" s="2"/>
+      <c r="G18" s="2"/>
+      <c r="H18" s="2"/>
+    </row>
+    <row r="19" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="1"/>
       <c r="B19" s="2"/>
       <c r="C19" s="2"/>
       <c r="D19" s="2"/>
-    </row>
-    <row r="20" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E19" s="2"/>
+      <c r="F19" s="2"/>
+      <c r="G19" s="2"/>
+      <c r="H19" s="2"/>
+    </row>
+    <row r="20" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="1"/>
       <c r="B20" s="2"/>
       <c r="C20" s="2"/>
       <c r="D20" s="2"/>
-    </row>
-    <row r="21" spans="1:4" ht="20" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="E20" s="2"/>
+      <c r="F20" s="2"/>
+      <c r="G20" s="2"/>
+    </row>
+    <row r="21" spans="1:8" ht="20" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="1"/>
       <c r="B21" s="2"/>
       <c r="C21" s="2"/>
       <c r="D21" s="2"/>
+      <c r="E21" s="2"/>
+      <c r="F21" s="2"/>
+      <c r="G21" s="2"/>
     </row>
   </sheetData>
   <mergeCells count="3">

</xml_diff>